<commit_message>
feat(backend): disable feedback by default and improve database connection handling
- Change default feedback_enabled setting from True to False across all event endpoints
- Add SKIP_DB_ON_STARTUP configuration option to allow local preview without MongoDB Atlas
- Implement retry logic with exponential backoff for MongoDB connection attempts
- Add proper SSL/TLS certificate configuration using certifi for secure connections
- Enhance database connection with improved timeout and pool settings
- Pass event name parameter to certificate sending service for better email context
- Add test_connection.py utility for verifying database connectivity
- Update participants.xlsx with latest participant data
- Improve logging for feedback_enabled status during certificate sending process
</commit_message>
<xml_diff>
--- a/participants/participants.xlsx
+++ b/participants/participants.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -426,9 +426,17 @@
         <v>1si23ad016@sit.ac.in</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Suraj Kumar</v>
+      </c>
+      <c r="B4" t="str">
+        <v>1si23ad057@sit.ac.in</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:B4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>